<commit_message>
6.8 Add Investigate Panel2
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/StoryScript11.xlsx
+++ b/Assets/StreamingAssets/StoryScript11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4C690C-50B6-E045-8A59-DC2A4CC57173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C651DD1A-4A2B-544E-9B5E-7AACEBB937CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" xr2:uid="{68C9ECD6-F2C7-A34A-8665-FFA8663C762C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="93">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,10 +118,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Question-Meeting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Question</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -403,13 +399,20 @@
   <si>
     <t>StoryScript12</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeetingRoom-Night</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Everyone left the banquet hall, each lost in their own thoughts.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -422,6 +425,14 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -460,7 +471,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -472,6 +483,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EEC272-F350-D34D-A243-3179172F76FB}">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -878,16 +892,16 @@
     </row>
     <row r="2" spans="1:16" ht="34">
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
         <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>19</v>
@@ -896,7 +910,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>19</v>
@@ -905,24 +919,24 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -936,16 +950,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -956,13 +970,13 @@
     </row>
     <row r="5" spans="1:16" ht="51">
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -973,13 +987,13 @@
     </row>
     <row r="6" spans="1:16" ht="34">
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -990,19 +1004,19 @@
     </row>
     <row r="7" spans="1:16" ht="34">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1016,16 +1030,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1036,13 +1050,13 @@
     </row>
     <row r="9" spans="1:16" ht="51">
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1053,13 +1067,13 @@
     </row>
     <row r="10" spans="1:16" ht="51">
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1070,13 +1084,13 @@
     </row>
     <row r="11" spans="1:16" ht="51">
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1087,19 +1101,19 @@
     </row>
     <row r="12" spans="1:16" ht="17">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1110,19 +1124,19 @@
     </row>
     <row r="13" spans="1:16" ht="17">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1133,19 +1147,19 @@
     </row>
     <row r="14" spans="1:16" ht="51">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1159,16 +1173,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1179,19 +1193,19 @@
     </row>
     <row r="16" spans="1:16" ht="34">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1205,16 +1219,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>19</v>
@@ -1223,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1234,16 +1248,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1254,19 +1268,19 @@
     </row>
     <row r="19" spans="1:12" ht="17">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1278,24 +1292,24 @@
         <v>0</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="34">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1306,19 +1320,19 @@
     </row>
     <row r="21" spans="1:12" ht="34">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1329,19 +1343,19 @@
     </row>
     <row r="22" spans="1:12" ht="51">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1355,16 +1369,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>14</v>
@@ -1379,13 +1393,13 @@
     </row>
     <row r="24" spans="1:12" ht="51">
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1399,16 +1413,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>19</v>
@@ -1417,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1425,19 +1439,19 @@
     </row>
     <row r="26" spans="1:12" ht="34">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1449,24 +1463,24 @@
         <v>0</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="34">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>14</v>
@@ -1474,20 +1488,20 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" ht="17">
-      <c r="B28" s="1" t="s">
-        <v>58</v>
+    <row r="28" spans="1:12" ht="34">
+      <c r="B28" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D28" t="s">
         <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -1497,81 +1511,75 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" ht="17">
-      <c r="A29" t="s">
-        <v>22</v>
-      </c>
       <c r="B29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
       </c>
       <c r="E29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" ht="17">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" t="s">
         <v>86</v>
       </c>
-      <c r="F29" t="s">
-        <v>87</v>
-      </c>
-      <c r="G29" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H30" s="3">
         <v>0</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J29" s="2" t="s">
+      <c r="I30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K30" s="2">
         <v>0</v>
       </c>
-      <c r="L29" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="34">
-      <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="L30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D30" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" t="s">
-        <v>85</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:12" ht="34">
       <c r="A31" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -1585,16 +1593,16 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -1603,21 +1611,21 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" ht="17">
+    <row r="33" spans="1:12" ht="34">
       <c r="A33" t="s">
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -1626,21 +1634,21 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" ht="34">
+    <row r="34" spans="1:12" ht="17">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="D34" t="s">
         <v>13</v>
       </c>
       <c r="E34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -1651,19 +1659,19 @@
     </row>
     <row r="35" spans="1:12" ht="34">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -1672,12 +1680,12 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" ht="17">
+    <row r="36" spans="1:12" ht="34">
       <c r="A36" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
         <v>76</v>
@@ -1686,7 +1694,7 @@
         <v>13</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -1697,19 +1705,19 @@
     </row>
     <row r="37" spans="1:12" ht="17">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D37" t="s">
         <v>13</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -1718,21 +1726,21 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" ht="51">
+    <row r="38" spans="1:12" ht="17">
       <c r="A38" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="D38" t="s">
         <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -1741,15 +1749,21 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" ht="17">
+    <row r="39" spans="1:12" ht="51">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
       <c r="B39" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
       </c>
       <c r="E39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -1758,15 +1772,15 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" ht="34">
+    <row r="40" spans="1:12" ht="17">
       <c r="B40" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
       </c>
       <c r="E40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -1776,20 +1790,14 @@
       <c r="L40" s="2"/>
     </row>
     <row r="41" spans="1:12" ht="34">
-      <c r="A41" t="s">
-        <v>22</v>
-      </c>
       <c r="B41" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
       </c>
       <c r="E41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -1798,21 +1806,21 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" ht="17">
+    <row r="42" spans="1:12" ht="34">
       <c r="A42" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="D42" t="s">
         <v>13</v>
       </c>
       <c r="E42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -1821,21 +1829,21 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" ht="34">
+    <row r="43" spans="1:12" ht="17">
       <c r="A43" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D43" t="s">
         <v>13</v>
       </c>
       <c r="E43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -1849,16 +1857,16 @@
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -1872,16 +1880,16 @@
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="D45" t="s">
         <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -1890,21 +1898,21 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" ht="17">
+    <row r="46" spans="1:12" ht="34">
       <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" t="s">
-        <v>80</v>
-      </c>
       <c r="D46" t="s">
         <v>13</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -1915,27 +1923,50 @@
     </row>
     <row r="47" spans="1:12" ht="17">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>91</v>
+        <v>72</v>
+      </c>
+      <c r="C47" t="s">
+        <v>79</v>
       </c>
       <c r="D47" t="s">
         <v>13</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
-      <c r="J47" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" ht="17">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
+        <v>84</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>